<commit_message>
pacific cross master plan created
</commit_message>
<xml_diff>
--- a/Inputs/Pacific_Cross_Master_Series/addons.xlsx
+++ b/Inputs/Pacific_Cross_Master_Series/addons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Dental" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="44">
   <si>
     <t xml:space="preserve">sheetName</t>
   </si>
@@ -206,11 +206,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -225,6 +221,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -328,11 +329,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -360,14 +361,14 @@
   </sheetPr>
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.30859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.31640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="71.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="71.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="11.52"/>
@@ -429,12 +430,15 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="I2" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -465,7 +469,7 @@
       <c r="A4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -493,15 +497,15 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
       <c r="E5" s="4"/>
       <c r="F5" s="2"/>
       <c r="H5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="4"/>
       <c r="F6" s="2"/>
       <c r="H6" s="5"/>
@@ -524,11 +528,11 @@
   </sheetPr>
   <dimension ref="A1:AA10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.12"/>
@@ -565,7 +569,7 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="T1" s="1"/>
@@ -575,11 +579,11 @@
       <c r="X1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="25.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -601,6 +605,9 @@
       <c r="H2" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="J2" s="0" t="s">
         <v>26</v>
@@ -613,11 +620,11 @@
       <c r="Y2" s="11"/>
       <c r="AA2" s="9"/>
     </row>
-    <row r="3" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="25.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -639,6 +646,9 @@
       <c r="H3" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="J3" s="0" t="s">
         <v>28</v>
@@ -651,11 +661,11 @@
       <c r="Y3" s="11"/>
       <c r="AA3" s="9"/>
     </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="25.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -678,25 +688,25 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="I4" s="0" t="s">
+        <v>18</v>
+      </c>
       <c r="J4" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="0" t="s">
-        <v>18</v>
-      </c>
       <c r="T4" s="9"/>
-      <c r="U4" s="8"/>
+      <c r="U4" s="7"/>
       <c r="V4" s="5"/>
       <c r="W4" s="2"/>
       <c r="X4" s="5"/>
       <c r="Y4" s="11"/>
       <c r="AA4" s="9"/>
     </row>
-    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="25.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -719,14 +729,14 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="I5" s="0" t="s">
+        <v>18</v>
+      </c>
       <c r="J5" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="0" t="s">
-        <v>18</v>
-      </c>
       <c r="T5" s="9"/>
-      <c r="U5" s="8"/>
+      <c r="U5" s="7"/>
       <c r="V5" s="5"/>
       <c r="W5" s="2"/>
       <c r="X5" s="5"/>
@@ -735,7 +745,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="T6" s="9"/>
-      <c r="U6" s="8"/>
+      <c r="U6" s="7"/>
       <c r="V6" s="5"/>
       <c r="W6" s="2"/>
       <c r="X6" s="5"/>
@@ -744,7 +754,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="T7" s="9"/>
-      <c r="U7" s="8"/>
+      <c r="U7" s="7"/>
       <c r="V7" s="5"/>
       <c r="W7" s="2"/>
       <c r="X7" s="5"/>
@@ -753,7 +763,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="T8" s="9"/>
-      <c r="U8" s="8"/>
+      <c r="U8" s="7"/>
       <c r="V8" s="5"/>
       <c r="W8" s="2"/>
       <c r="X8" s="5"/>
@@ -762,7 +772,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="T9" s="9"/>
-      <c r="U9" s="8"/>
+      <c r="U9" s="7"/>
       <c r="V9" s="5"/>
       <c r="W9" s="2"/>
       <c r="X9" s="5"/>
@@ -771,7 +781,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="T10" s="9"/>
-      <c r="U10" s="8"/>
+      <c r="U10" s="7"/>
       <c r="V10" s="5"/>
       <c r="W10" s="2"/>
       <c r="X10" s="5"/>
@@ -800,7 +810,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -866,10 +876,10 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.12"/>
@@ -928,7 +938,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -953,7 +963,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -999,7 +1009,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.12"/>
@@ -1051,7 +1061,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1073,7 +1083,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1116,11 +1126,11 @@
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.08"/>
   </cols>
@@ -1168,7 +1178,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1190,7 +1200,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1229,11 +1239,11 @@
   </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>